<commit_message>
Jobsheet8_Tugas1_Implementasi Upload file untuk import data pada semua menu
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +447,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>

</xml_diff>